<commit_message>
Feat: Complete Final stock-check flow
</commit_message>
<xml_diff>
--- a/src/assets/export-templates/template_xuat_noi_bo.xlsx
+++ b/src/assets/export-templates/template_xuat_noi_bo.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CAPSTONE\warehouse_frontend\src\assets\export-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3873D4F-5AEE-458D-9D0E-70E225E5186A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD30744-F0E8-4D68-99B0-6DE46FB880A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{9FA52C3A-7928-408F-877C-18AC7D4D703A}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="28800" windowHeight="15370" xr2:uid="{9FA52C3A-7928-408F-877C-18AC7D4D703A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template xuất sản xuất" sheetId="2" r:id="rId1"/>
+    <sheet name="Template xuất nội bộ" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -233,22 +233,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -656,7 +656,7 @@
   <dimension ref="A1:BM200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>